<commit_message>
Bug fixes related to Google Chrome version
</commit_message>
<xml_diff>
--- a/OutputData.xlsx
+++ b/OutputData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="48">
   <si>
     <t>User</t>
   </si>
@@ -500,7 +500,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1134,6 +1134,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45"/>
+      <c r="B45"/>
+      <c r="C45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>